<commit_message>
set Pivot Value Field Format to # ##,00
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/PivotTable.xlsx
+++ b/src/main/resources/xlsx/PivotTable.xlsx
@@ -154,7 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,7 +370,7 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of balance" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of balance" fld="4" baseField="0" baseItem="0" numFmtId="4"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -661,15 +661,15 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
set Pivot Value Field Format to # ##0
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/PivotTable.xlsx
+++ b/src/main/resources/xlsx/PivotTable.xlsx
@@ -145,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -155,11 +155,16 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -372,6 +377,11 @@
   <dataFields count="1">
     <dataField name="Sum of balance" fld="4" baseField="0" baseItem="0" numFmtId="4"/>
   </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -661,7 +671,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -938,7 +948,7 @@
       <c r="I14" s="4">
         <v>19742.57</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="5">
         <v>33832.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
set Pivot Value Field Format to # ##?/?
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/PivotTable.xlsx
+++ b/src/main/resources/xlsx/PivotTable.xlsx
@@ -117,6 +117,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -145,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -154,15 +157,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -375,11 +386,20 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of balance" fld="4" baseField="0" baseItem="0" numFmtId="4"/>
+    <dataField name="Sum of balance" fld="4" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
-  <formats count="1">
+  <formats count="2">
+    <format dxfId="3">
+      <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
     <format dxfId="0">
-      <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -671,7 +691,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,7 +968,7 @@
       <c r="I14" s="4">
         <v>19742.57</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="4">
         <v>33832.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pivot Field subtotal off
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/PivotTable.xlsx
+++ b/src/main/resources/xlsx/PivotTable.xlsx
@@ -162,7 +162,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
     </dxf>
@@ -295,12 +301,11 @@
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G3:J14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="3">
         <item x="2"/>
         <item x="1"/>
         <item x="0"/>
-        <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
@@ -389,10 +394,10 @@
     <dataField name="Sum of balance" fld="4" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="3">
+    <format dxfId="5">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="2">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -691,7 +696,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -807,13 +812,9 @@
       <c r="G5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="4">
-        <v>8923.34</v>
-      </c>
+      <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4">
-        <v>8923.34</v>
-      </c>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -862,12 +863,8 @@
         <v>17</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="4">
-        <v>2343.9</v>
-      </c>
-      <c r="J7" s="4">
-        <v>2343.9</v>
-      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -900,15 +897,9 @@
       <c r="G9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="4">
-        <v>5166.59</v>
-      </c>
-      <c r="I9" s="4">
-        <v>17398.669999999998</v>
-      </c>
-      <c r="J9" s="4">
-        <v>22565.260000000002</v>
-      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G10" s="3" t="s">

</xml_diff>

<commit_message>
create CustomPivotTable.java and  NumFmtId=14
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/PivotTable.xlsx
+++ b/src/main/resources/xlsx/PivotTable.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="20" r:id="rId2"/>
+    <pivotCache cacheId="50" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -148,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -158,25 +158,14 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#\ ##?/?"/>
@@ -298,7 +287,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="50" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G3:J14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
@@ -394,10 +383,10 @@
     <dataField name="Sum of balance" fld="4" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="5">
+    <format dxfId="1">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -696,7 +685,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,6 +903,9 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D11" s="5">
+        <v>42016</v>
+      </c>
       <c r="G11" s="3" t="s">
         <v>12</v>
       </c>

</xml_diff>